<commit_message>
update revision, and some other things since losing laptop
</commit_message>
<xml_diff>
--- a/Data/Static Data.xlsx
+++ b/Data/Static Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Semester 7\Seminar - Skripsi\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismi\Downloads\skripsi-zaka\seminar-skripsi-master\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Static Data x" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Real</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>x Error</t>
+  </si>
+  <si>
+    <t>y Error</t>
+  </si>
+  <si>
+    <t>z Error</t>
   </si>
 </sst>
 </file>
@@ -790,7 +799,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -912,7 +921,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1034,7 +1043,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1157,16 +1166,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="113894080"/>
-        <c:axId val="114068896"/>
+        <c:axId val="394507032"/>
+        <c:axId val="394507424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113894080"/>
+        <c:axId val="394507032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID"/>
+                  <a:t>object posistion in real x axis (CM)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1204,7 +1269,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114068896"/>
+        <c:crossAx val="394507424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1212,7 +1277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114068896"/>
+        <c:axId val="394507424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,6 +1311,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800"/>
+                  <a:t>system estimation error</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" baseline="0"/>
+                  <a:t> (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1277,7 +1403,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113894080"/>
+        <c:crossAx val="394507032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1387,7 +1513,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1521,7 +1647,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1655,7 +1781,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1790,16 +1916,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="113837760"/>
-        <c:axId val="205485824"/>
+        <c:axId val="394508208"/>
+        <c:axId val="394508600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113837760"/>
+        <c:axId val="394508208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="900" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real x axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1837,7 +2024,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205485824"/>
+        <c:crossAx val="394508600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1845,7 +2032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205485824"/>
+        <c:axId val="394508600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,6 +2066,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="100">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1910,7 +2158,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113837760"/>
+        <c:crossAx val="394508208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2020,7 +2268,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2178,7 +2426,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2336,7 +2584,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2495,16 +2743,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="111346528"/>
-        <c:axId val="111347088"/>
+        <c:axId val="248892464"/>
+        <c:axId val="248892856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111346528"/>
+        <c:axId val="248892464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="900" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real x axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2542,7 +2851,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111347088"/>
+        <c:crossAx val="248892856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2550,7 +2859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111347088"/>
+        <c:axId val="248892856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2584,6 +2893,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="100">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2615,7 +2985,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111346528"/>
+        <c:crossAx val="248892464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2725,7 +3095,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2895,7 +3265,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3065,7 +3435,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3236,16 +3606,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="111351008"/>
-        <c:axId val="111351568"/>
+        <c:axId val="248893640"/>
+        <c:axId val="248894032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111351008"/>
+        <c:axId val="248893640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="900" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real x axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3283,7 +3714,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111351568"/>
+        <c:crossAx val="248894032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3291,7 +3722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111351568"/>
+        <c:axId val="248894032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3325,6 +3756,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="100">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3356,7 +3848,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111351008"/>
+        <c:crossAx val="248893640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3466,7 +3958,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3636,7 +4128,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3806,7 +4298,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3977,16 +4469,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="205638608"/>
-        <c:axId val="206039920"/>
+        <c:axId val="248894816"/>
+        <c:axId val="248895208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="205638608"/>
+        <c:axId val="248894816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="900" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real x axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4024,7 +4577,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206039920"/>
+        <c:crossAx val="248895208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4032,7 +4585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206039920"/>
+        <c:axId val="248895208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4066,6 +4619,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="100">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4097,7 +4711,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205638608"/>
+        <c:crossAx val="248894816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4207,7 +4821,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4353,7 +4967,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4499,7 +5113,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4646,16 +5260,77 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="257198240"/>
-        <c:axId val="253933696"/>
+        <c:axId val="248895992"/>
+        <c:axId val="248896384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="257198240"/>
+        <c:axId val="248895992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real Y axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4693,7 +5368,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253933696"/>
+        <c:crossAx val="248896384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4701,17 +5376,105 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253933696"/>
+        <c:axId val="248896384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="900" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="300">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257198240"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="248895992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4821,7 +5584,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4967,7 +5730,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5113,7 +5876,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5260,16 +6023,77 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="254974464"/>
-        <c:axId val="254975024"/>
+        <c:axId val="248897168"/>
+        <c:axId val="248897560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="254974464"/>
+        <c:axId val="248897168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real Y axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5307,7 +6131,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254975024"/>
+        <c:crossAx val="248897560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5315,17 +6139,105 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254975024"/>
+        <c:axId val="248897560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254974464"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="248897168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5435,7 +6347,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>x</c:v>
+                  <c:v>x Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5581,7 +6493,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>y Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5727,7 +6639,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>z Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5874,16 +6786,77 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="253974272"/>
-        <c:axId val="253971472"/>
+        <c:axId val="248898344"/>
+        <c:axId val="248898736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="253974272"/>
+        <c:axId val="248898344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>object posistion in real x axis (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5921,7 +6894,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253971472"/>
+        <c:crossAx val="248898736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5929,17 +6902,105 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253971472"/>
+        <c:axId val="248898736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="id-ID" sz="800" b="0" i="0" cap="all" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>system estimation error (CM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="id-ID" sz="200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="id-ID"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="253974272"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="248898344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10876,8 +11937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:I17"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10919,13 +11980,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -12467,8 +13528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12510,13 +13571,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>